<commit_message>
Resources operational in all software + correction of climate change damage indicators fate factors.
</commit_message>
<xml_diff>
--- a/Data/mappings/exiobase/EXIO_3_8_IW_concordance.xlsx
+++ b/Data/mappings/exiobase/EXIO_3_8_IW_concordance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\exiobase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3DE245-0711-4A17-9812-A431D13376B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D3F5E2-363A-4B6A-AA6E-22F111021766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="1154">
   <si>
     <t>Taxes less subsidies on products purchased: Total</t>
   </si>
@@ -3402,15 +3402,6 @@
   </si>
   <si>
     <t>Phosphorus</t>
-  </si>
-  <si>
-    <t>Wood, soft, standing</t>
-  </si>
-  <si>
-    <t>Wood, hard, standing</t>
-  </si>
-  <si>
-    <t>Coal, brown</t>
   </si>
   <si>
     <t>Carbon dioxide, fossil</t>
@@ -3594,10 +3585,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3866,7 +3853,7 @@
   <dimension ref="A1:B1114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3895,17 +3882,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4003,7 +3990,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -4051,7 +4038,7 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -4147,7 +4134,7 @@
         <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -4155,7 +4142,7 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -4163,7 +4150,7 @@
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -4171,7 +4158,7 @@
         <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -4179,7 +4166,7 @@
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -4187,7 +4174,7 @@
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -4195,7 +4182,7 @@
         <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -4203,7 +4190,7 @@
         <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -4211,7 +4198,7 @@
         <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -4219,7 +4206,7 @@
         <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -4227,7 +4214,7 @@
         <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -4235,7 +4222,7 @@
         <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -4243,7 +4230,7 @@
         <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -4251,7 +4238,7 @@
         <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -4259,7 +4246,7 @@
         <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -4267,7 +4254,7 @@
         <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -4275,7 +4262,7 @@
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -4419,7 +4406,7 @@
         <v>72</v>
       </c>
       <c r="B77" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -4427,7 +4414,7 @@
         <v>73</v>
       </c>
       <c r="B78" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -4435,7 +4422,7 @@
         <v>74</v>
       </c>
       <c r="B79" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -4443,7 +4430,7 @@
         <v>75</v>
       </c>
       <c r="B80" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -4451,7 +4438,7 @@
         <v>76</v>
       </c>
       <c r="B81" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -4459,7 +4446,7 @@
         <v>77</v>
       </c>
       <c r="B82" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -4467,7 +4454,7 @@
         <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -4475,7 +4462,7 @@
         <v>79</v>
       </c>
       <c r="B84" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -4483,7 +4470,7 @@
         <v>80</v>
       </c>
       <c r="B85" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -4491,7 +4478,7 @@
         <v>81</v>
       </c>
       <c r="B86" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -4499,7 +4486,7 @@
         <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -4507,7 +4494,7 @@
         <v>83</v>
       </c>
       <c r="B88" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -4515,7 +4502,7 @@
         <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -4523,7 +4510,7 @@
         <v>85</v>
       </c>
       <c r="B90" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -4531,7 +4518,7 @@
         <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -4539,7 +4526,7 @@
         <v>87</v>
       </c>
       <c r="B92" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -4547,7 +4534,7 @@
         <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -4555,7 +4542,7 @@
         <v>89</v>
       </c>
       <c r="B94" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -4563,7 +4550,7 @@
         <v>90</v>
       </c>
       <c r="B95" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -4571,7 +4558,7 @@
         <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -4579,7 +4566,7 @@
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -4587,7 +4574,7 @@
         <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -4595,7 +4582,7 @@
         <v>94</v>
       </c>
       <c r="B99" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -4603,7 +4590,7 @@
         <v>95</v>
       </c>
       <c r="B100" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -4611,7 +4598,7 @@
         <v>96</v>
       </c>
       <c r="B101" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -4619,7 +4606,7 @@
         <v>97</v>
       </c>
       <c r="B102" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -4627,7 +4614,7 @@
         <v>98</v>
       </c>
       <c r="B103" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -4635,7 +4622,7 @@
         <v>99</v>
       </c>
       <c r="B104" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -4643,7 +4630,7 @@
         <v>100</v>
       </c>
       <c r="B105" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -4651,7 +4638,7 @@
         <v>101</v>
       </c>
       <c r="B106" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -4659,7 +4646,7 @@
         <v>102</v>
       </c>
       <c r="B107" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -4667,7 +4654,7 @@
         <v>103</v>
       </c>
       <c r="B108" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -4675,7 +4662,7 @@
         <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -4683,7 +4670,7 @@
         <v>105</v>
       </c>
       <c r="B110" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -4691,7 +4678,7 @@
         <v>106</v>
       </c>
       <c r="B111" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -4699,7 +4686,7 @@
         <v>107</v>
       </c>
       <c r="B112" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -4707,7 +4694,7 @@
         <v>108</v>
       </c>
       <c r="B113" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -4715,7 +4702,7 @@
         <v>109</v>
       </c>
       <c r="B114" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -4723,7 +4710,7 @@
         <v>110</v>
       </c>
       <c r="B115" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -4731,7 +4718,7 @@
         <v>111</v>
       </c>
       <c r="B116" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -4739,7 +4726,7 @@
         <v>112</v>
       </c>
       <c r="B117" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -4747,7 +4734,7 @@
         <v>113</v>
       </c>
       <c r="B118" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -4755,7 +4742,7 @@
         <v>114</v>
       </c>
       <c r="B119" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -4763,7 +4750,7 @@
         <v>115</v>
       </c>
       <c r="B120" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -4771,7 +4758,7 @@
         <v>116</v>
       </c>
       <c r="B121" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -4779,7 +4766,7 @@
         <v>117</v>
       </c>
       <c r="B122" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -4803,7 +4790,7 @@
         <v>120</v>
       </c>
       <c r="B125" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -4811,7 +4798,7 @@
         <v>121</v>
       </c>
       <c r="B126" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
@@ -4819,7 +4806,7 @@
         <v>122</v>
       </c>
       <c r="B127" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -4827,7 +4814,7 @@
         <v>123</v>
       </c>
       <c r="B128" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -4835,7 +4822,7 @@
         <v>124</v>
       </c>
       <c r="B129" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -4843,7 +4830,7 @@
         <v>125</v>
       </c>
       <c r="B130" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -4851,7 +4838,7 @@
         <v>126</v>
       </c>
       <c r="B131" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -4859,7 +4846,7 @@
         <v>127</v>
       </c>
       <c r="B132" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -4867,7 +4854,7 @@
         <v>128</v>
       </c>
       <c r="B133" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -4883,7 +4870,7 @@
         <v>130</v>
       </c>
       <c r="B135" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -4891,7 +4878,7 @@
         <v>131</v>
       </c>
       <c r="B136" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -4899,7 +4886,7 @@
         <v>132</v>
       </c>
       <c r="B137" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -4907,7 +4894,7 @@
         <v>133</v>
       </c>
       <c r="B138" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
@@ -5499,7 +5486,7 @@
         <v>207</v>
       </c>
       <c r="B212" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
@@ -5507,7 +5494,7 @@
         <v>208</v>
       </c>
       <c r="B213" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -5515,7 +5502,7 @@
         <v>209</v>
       </c>
       <c r="B214" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
@@ -5523,7 +5510,7 @@
         <v>210</v>
       </c>
       <c r="B215" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -5531,7 +5518,7 @@
         <v>211</v>
       </c>
       <c r="B216" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
@@ -5539,7 +5526,7 @@
         <v>212</v>
       </c>
       <c r="B217" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
@@ -5547,7 +5534,7 @@
         <v>213</v>
       </c>
       <c r="B218" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
@@ -5555,7 +5542,7 @@
         <v>214</v>
       </c>
       <c r="B219" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
@@ -6443,7 +6430,7 @@
         <v>325</v>
       </c>
       <c r="B330" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
@@ -6451,7 +6438,7 @@
         <v>326</v>
       </c>
       <c r="B331" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
@@ -6459,7 +6446,7 @@
         <v>327</v>
       </c>
       <c r="B332" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
@@ -6467,7 +6454,7 @@
         <v>328</v>
       </c>
       <c r="B333" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
@@ -6475,7 +6462,7 @@
         <v>329</v>
       </c>
       <c r="B334" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
@@ -6483,7 +6470,7 @@
         <v>330</v>
       </c>
       <c r="B335" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
@@ -6491,7 +6478,7 @@
         <v>331</v>
       </c>
       <c r="B336" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
@@ -6499,7 +6486,7 @@
         <v>332</v>
       </c>
       <c r="B337" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
@@ -6507,7 +6494,7 @@
         <v>333</v>
       </c>
       <c r="B338" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
@@ -6515,7 +6502,7 @@
         <v>334</v>
       </c>
       <c r="B339" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
@@ -6523,7 +6510,7 @@
         <v>335</v>
       </c>
       <c r="B340" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
@@ -6531,7 +6518,7 @@
         <v>336</v>
       </c>
       <c r="B341" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
@@ -6539,7 +6526,7 @@
         <v>337</v>
       </c>
       <c r="B342" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
@@ -6547,7 +6534,7 @@
         <v>338</v>
       </c>
       <c r="B343" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
@@ -6707,7 +6694,7 @@
         <v>358</v>
       </c>
       <c r="B363" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
@@ -6715,7 +6702,7 @@
         <v>359</v>
       </c>
       <c r="B364" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
@@ -6723,7 +6710,7 @@
         <v>360</v>
       </c>
       <c r="B365" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
@@ -6731,7 +6718,7 @@
         <v>361</v>
       </c>
       <c r="B366" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
@@ -7107,7 +7094,7 @@
         <v>408</v>
       </c>
       <c r="B413" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.3">
@@ -7115,7 +7102,7 @@
         <v>409</v>
       </c>
       <c r="B414" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.3">
@@ -7123,7 +7110,7 @@
         <v>410</v>
       </c>
       <c r="B415" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
@@ -7131,7 +7118,7 @@
         <v>411</v>
       </c>
       <c r="B416" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.3">
@@ -7139,7 +7126,7 @@
         <v>412</v>
       </c>
       <c r="B417" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.3">
@@ -7147,7 +7134,7 @@
         <v>413</v>
       </c>
       <c r="B418" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.3">
@@ -7155,7 +7142,7 @@
         <v>414</v>
       </c>
       <c r="B419" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.3">
@@ -7163,7 +7150,7 @@
         <v>415</v>
       </c>
       <c r="B420" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.3">
@@ -7171,7 +7158,7 @@
         <v>416</v>
       </c>
       <c r="B421" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.3">
@@ -7179,7 +7166,7 @@
         <v>417</v>
       </c>
       <c r="B422" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.3">
@@ -7187,7 +7174,7 @@
         <v>418</v>
       </c>
       <c r="B423" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.3">
@@ -7195,7 +7182,7 @@
         <v>419</v>
       </c>
       <c r="B424" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.3">
@@ -7211,7 +7198,7 @@
         <v>421</v>
       </c>
       <c r="B426" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.3">
@@ -7219,7 +7206,7 @@
         <v>422</v>
       </c>
       <c r="B427" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.3">
@@ -7235,7 +7222,7 @@
         <v>424</v>
       </c>
       <c r="B429" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.3">
@@ -7243,7 +7230,7 @@
         <v>425</v>
       </c>
       <c r="B430" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.3">
@@ -7301,7 +7288,7 @@
         <v>433</v>
       </c>
       <c r="B438" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.3">
@@ -7309,7 +7296,7 @@
         <v>434</v>
       </c>
       <c r="B439" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.3">
@@ -7317,7 +7304,7 @@
         <v>435</v>
       </c>
       <c r="B440" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.3">
@@ -7330,7 +7317,7 @@
         <v>437</v>
       </c>
       <c r="B442" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.3">
@@ -7378,7 +7365,7 @@
         <v>443</v>
       </c>
       <c r="B448" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.3">
@@ -7386,7 +7373,7 @@
         <v>444</v>
       </c>
       <c r="B449" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.3">
@@ -7394,7 +7381,7 @@
         <v>445</v>
       </c>
       <c r="B450" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.3">
@@ -7402,7 +7389,7 @@
         <v>446</v>
       </c>
       <c r="B451" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.3">
@@ -7410,7 +7397,7 @@
         <v>447</v>
       </c>
       <c r="B452" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.3">
@@ -7418,7 +7405,7 @@
         <v>448</v>
       </c>
       <c r="B453" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.3">
@@ -7426,7 +7413,7 @@
         <v>449</v>
       </c>
       <c r="B454" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.3">
@@ -7434,7 +7421,7 @@
         <v>450</v>
       </c>
       <c r="B455" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.3">
@@ -7442,7 +7429,7 @@
         <v>451</v>
       </c>
       <c r="B456" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.3">
@@ -7450,7 +7437,7 @@
         <v>452</v>
       </c>
       <c r="B457" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.3">
@@ -7458,7 +7445,7 @@
         <v>453</v>
       </c>
       <c r="B458" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.3">
@@ -7466,7 +7453,7 @@
         <v>454</v>
       </c>
       <c r="B459" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.3">
@@ -7474,7 +7461,7 @@
         <v>455</v>
       </c>
       <c r="B460" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.3">
@@ -7482,7 +7469,7 @@
         <v>456</v>
       </c>
       <c r="B461" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.3">
@@ -7490,7 +7477,7 @@
         <v>457</v>
       </c>
       <c r="B462" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.3">
@@ -7498,7 +7485,7 @@
         <v>458</v>
       </c>
       <c r="B463" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.3">
@@ -7506,7 +7493,7 @@
         <v>459</v>
       </c>
       <c r="B464" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.3">
@@ -7514,7 +7501,7 @@
         <v>460</v>
       </c>
       <c r="B465" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.3">
@@ -7522,7 +7509,7 @@
         <v>461</v>
       </c>
       <c r="B466" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.3">
@@ -7530,7 +7517,7 @@
         <v>462</v>
       </c>
       <c r="B467" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.3">
@@ -7578,7 +7565,7 @@
         <v>471</v>
       </c>
       <c r="B476" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.3">
@@ -7586,7 +7573,7 @@
         <v>472</v>
       </c>
       <c r="B477" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.3">
@@ -7604,177 +7591,162 @@
         <v>475</v>
       </c>
     </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A481" s="2" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A482" s="2" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A483" s="2" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A484" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A485" s="2" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A486" s="2" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A487" s="2" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A488" s="2" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A489" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A490" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A491" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A492" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A493" s="2" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A494" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="B494" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A495" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="B495" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A496" s="2" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A497" s="2" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A498" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B498" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A499" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="B499" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A500" s="2" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="501" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A501" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="B501" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="502" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A502" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="503" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A503" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="504" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A504" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="505" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A505" s="2" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="506" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A506" s="2" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="507" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A507" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="508" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A508" s="2" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="509" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A509" s="2" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="510" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A510" s="2" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="511" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A511" s="2" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="512" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A512" s="2" t="s">
         <v>507</v>
       </c>
@@ -9844,7 +9816,7 @@
         <v>920</v>
       </c>
       <c r="B925" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.3">
@@ -9852,7 +9824,7 @@
         <v>921</v>
       </c>
       <c r="B926" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.3">
@@ -9860,7 +9832,7 @@
         <v>922</v>
       </c>
       <c r="B927" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.3">
@@ -9868,7 +9840,7 @@
         <v>923</v>
       </c>
       <c r="B928" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.3">
@@ -9876,7 +9848,7 @@
         <v>924</v>
       </c>
       <c r="B929" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.3">
@@ -9884,7 +9856,7 @@
         <v>925</v>
       </c>
       <c r="B930" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.3">
@@ -9892,7 +9864,7 @@
         <v>926</v>
       </c>
       <c r="B931" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.3">
@@ -9900,7 +9872,7 @@
         <v>927</v>
       </c>
       <c r="B932" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.3">
@@ -9908,7 +9880,7 @@
         <v>928</v>
       </c>
       <c r="B933" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.3">
@@ -9916,7 +9888,7 @@
         <v>929</v>
       </c>
       <c r="B934" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.3">
@@ -9924,7 +9896,7 @@
         <v>930</v>
       </c>
       <c r="B935" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.3">
@@ -9932,7 +9904,7 @@
         <v>931</v>
       </c>
       <c r="B936" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.3">
@@ -9940,7 +9912,7 @@
         <v>932</v>
       </c>
       <c r="B937" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.3">
@@ -9948,7 +9920,7 @@
         <v>933</v>
       </c>
       <c r="B938" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.3">
@@ -9956,7 +9928,7 @@
         <v>934</v>
       </c>
       <c r="B939" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.3">
@@ -9964,7 +9936,7 @@
         <v>935</v>
       </c>
       <c r="B940" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.3">
@@ -9972,7 +9944,7 @@
         <v>936</v>
       </c>
       <c r="B941" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.3">
@@ -9980,7 +9952,7 @@
         <v>937</v>
       </c>
       <c r="B942" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.3">
@@ -9988,7 +9960,7 @@
         <v>938</v>
       </c>
       <c r="B943" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.3">
@@ -9996,7 +9968,7 @@
         <v>939</v>
       </c>
       <c r="B944" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.3">
@@ -10004,7 +9976,7 @@
         <v>940</v>
       </c>
       <c r="B945" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.3">
@@ -10012,7 +9984,7 @@
         <v>941</v>
       </c>
       <c r="B946" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.3">
@@ -10020,7 +9992,7 @@
         <v>942</v>
       </c>
       <c r="B947" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.3">
@@ -10028,7 +10000,7 @@
         <v>943</v>
       </c>
       <c r="B948" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.3">
@@ -10036,7 +10008,7 @@
         <v>944</v>
       </c>
       <c r="B949" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.3">
@@ -10044,7 +10016,7 @@
         <v>945</v>
       </c>
       <c r="B950" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.3">
@@ -10052,7 +10024,7 @@
         <v>946</v>
       </c>
       <c r="B951" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.3">
@@ -10060,7 +10032,7 @@
         <v>947</v>
       </c>
       <c r="B952" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.3">
@@ -10068,7 +10040,7 @@
         <v>948</v>
       </c>
       <c r="B953" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.3">
@@ -10076,7 +10048,7 @@
         <v>949</v>
       </c>
       <c r="B954" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.3">
@@ -10084,7 +10056,7 @@
         <v>950</v>
       </c>
       <c r="B955" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.3">
@@ -10092,7 +10064,7 @@
         <v>951</v>
       </c>
       <c r="B956" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.3">
@@ -10100,7 +10072,7 @@
         <v>952</v>
       </c>
       <c r="B957" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.3">
@@ -10108,7 +10080,7 @@
         <v>953</v>
       </c>
       <c r="B958" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.3">
@@ -10116,7 +10088,7 @@
         <v>954</v>
       </c>
       <c r="B959" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.3">
@@ -10124,7 +10096,7 @@
         <v>955</v>
       </c>
       <c r="B960" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.3">
@@ -10132,7 +10104,7 @@
         <v>956</v>
       </c>
       <c r="B961" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.3">
@@ -10140,7 +10112,7 @@
         <v>957</v>
       </c>
       <c r="B962" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.3">
@@ -10148,7 +10120,7 @@
         <v>958</v>
       </c>
       <c r="B963" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.3">
@@ -10156,7 +10128,7 @@
         <v>959</v>
       </c>
       <c r="B964" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.3">
@@ -10164,7 +10136,7 @@
         <v>960</v>
       </c>
       <c r="B965" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.3">
@@ -10172,7 +10144,7 @@
         <v>961</v>
       </c>
       <c r="B966" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.3">
@@ -10180,7 +10152,7 @@
         <v>962</v>
       </c>
       <c r="B967" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.3">
@@ -10188,7 +10160,7 @@
         <v>963</v>
       </c>
       <c r="B968" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.3">
@@ -10196,7 +10168,7 @@
         <v>964</v>
       </c>
       <c r="B969" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.3">
@@ -10204,7 +10176,7 @@
         <v>965</v>
       </c>
       <c r="B970" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.3">
@@ -10212,7 +10184,7 @@
         <v>966</v>
       </c>
       <c r="B971" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.3">
@@ -10220,7 +10192,7 @@
         <v>967</v>
       </c>
       <c r="B972" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.3">
@@ -10228,7 +10200,7 @@
         <v>968</v>
       </c>
       <c r="B973" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.3">
@@ -10236,7 +10208,7 @@
         <v>969</v>
       </c>
       <c r="B974" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.3">
@@ -10244,7 +10216,7 @@
         <v>970</v>
       </c>
       <c r="B975" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.3">
@@ -10252,7 +10224,7 @@
         <v>971</v>
       </c>
       <c r="B976" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.3">
@@ -10260,7 +10232,7 @@
         <v>972</v>
       </c>
       <c r="B977" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.3">
@@ -10268,7 +10240,7 @@
         <v>973</v>
       </c>
       <c r="B978" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.3">
@@ -10276,7 +10248,7 @@
         <v>974</v>
       </c>
       <c r="B979" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.3">
@@ -10284,7 +10256,7 @@
         <v>975</v>
       </c>
       <c r="B980" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.3">
@@ -10292,7 +10264,7 @@
         <v>976</v>
       </c>
       <c r="B981" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.3">
@@ -10300,7 +10272,7 @@
         <v>977</v>
       </c>
       <c r="B982" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.3">
@@ -10308,7 +10280,7 @@
         <v>978</v>
       </c>
       <c r="B983" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.3">
@@ -10316,7 +10288,7 @@
         <v>979</v>
       </c>
       <c r="B984" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.3">
@@ -10324,7 +10296,7 @@
         <v>980</v>
       </c>
       <c r="B985" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.3">
@@ -10332,7 +10304,7 @@
         <v>981</v>
       </c>
       <c r="B986" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.3">
@@ -10340,7 +10312,7 @@
         <v>982</v>
       </c>
       <c r="B987" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.3">
@@ -10348,7 +10320,7 @@
         <v>983</v>
       </c>
       <c r="B988" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.3">
@@ -10356,7 +10328,7 @@
         <v>984</v>
       </c>
       <c r="B989" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.3">
@@ -10364,7 +10336,7 @@
         <v>985</v>
       </c>
       <c r="B990" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.3">
@@ -10372,7 +10344,7 @@
         <v>986</v>
       </c>
       <c r="B991" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.3">
@@ -10380,7 +10352,7 @@
         <v>987</v>
       </c>
       <c r="B992" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.3">
@@ -10388,7 +10360,7 @@
         <v>988</v>
       </c>
       <c r="B993" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.3">
@@ -10396,7 +10368,7 @@
         <v>989</v>
       </c>
       <c r="B994" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.3">
@@ -10404,7 +10376,7 @@
         <v>990</v>
       </c>
       <c r="B995" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.3">
@@ -10412,7 +10384,7 @@
         <v>991</v>
       </c>
       <c r="B996" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.3">
@@ -10420,7 +10392,7 @@
         <v>992</v>
       </c>
       <c r="B997" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.3">
@@ -10428,7 +10400,7 @@
         <v>993</v>
       </c>
       <c r="B998" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.3">
@@ -10436,7 +10408,7 @@
         <v>994</v>
       </c>
       <c r="B999" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1000" spans="1:2" x14ac:dyDescent="0.3">
@@ -10444,7 +10416,7 @@
         <v>995</v>
       </c>
       <c r="B1000" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1001" spans="1:2" x14ac:dyDescent="0.3">
@@ -10452,7 +10424,7 @@
         <v>996</v>
       </c>
       <c r="B1001" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1002" spans="1:2" x14ac:dyDescent="0.3">
@@ -10460,7 +10432,7 @@
         <v>997</v>
       </c>
       <c r="B1002" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1003" spans="1:2" x14ac:dyDescent="0.3">
@@ -10468,7 +10440,7 @@
         <v>998</v>
       </c>
       <c r="B1003" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.3">
@@ -10476,7 +10448,7 @@
         <v>999</v>
       </c>
       <c r="B1004" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1005" spans="1:2" x14ac:dyDescent="0.3">
@@ -10484,7 +10456,7 @@
         <v>1000</v>
       </c>
       <c r="B1005" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1006" spans="1:2" x14ac:dyDescent="0.3">
@@ -10492,7 +10464,7 @@
         <v>1001</v>
       </c>
       <c r="B1006" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1007" spans="1:2" x14ac:dyDescent="0.3">
@@ -10500,7 +10472,7 @@
         <v>1002</v>
       </c>
       <c r="B1007" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1008" spans="1:2" x14ac:dyDescent="0.3">
@@ -10508,7 +10480,7 @@
         <v>1003</v>
       </c>
       <c r="B1008" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1009" spans="1:2" x14ac:dyDescent="0.3">
@@ -10516,7 +10488,7 @@
         <v>1004</v>
       </c>
       <c r="B1009" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1010" spans="1:2" x14ac:dyDescent="0.3">
@@ -10524,7 +10496,7 @@
         <v>1005</v>
       </c>
       <c r="B1010" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1011" spans="1:2" x14ac:dyDescent="0.3">
@@ -10532,7 +10504,7 @@
         <v>1006</v>
       </c>
       <c r="B1011" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1012" spans="1:2" x14ac:dyDescent="0.3">
@@ -10540,7 +10512,7 @@
         <v>1007</v>
       </c>
       <c r="B1012" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1013" spans="1:2" x14ac:dyDescent="0.3">
@@ -10548,7 +10520,7 @@
         <v>1008</v>
       </c>
       <c r="B1013" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1014" spans="1:2" x14ac:dyDescent="0.3">
@@ -10556,7 +10528,7 @@
         <v>1009</v>
       </c>
       <c r="B1014" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1015" spans="1:2" x14ac:dyDescent="0.3">
@@ -10564,7 +10536,7 @@
         <v>1010</v>
       </c>
       <c r="B1015" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1016" spans="1:2" x14ac:dyDescent="0.3">
@@ -10572,7 +10544,7 @@
         <v>1011</v>
       </c>
       <c r="B1016" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1017" spans="1:2" x14ac:dyDescent="0.3">
@@ -10580,7 +10552,7 @@
         <v>1012</v>
       </c>
       <c r="B1017" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1018" spans="1:2" x14ac:dyDescent="0.3">
@@ -10588,7 +10560,7 @@
         <v>1013</v>
       </c>
       <c r="B1018" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1019" spans="1:2" x14ac:dyDescent="0.3">
@@ -10596,7 +10568,7 @@
         <v>1014</v>
       </c>
       <c r="B1019" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1020" spans="1:2" x14ac:dyDescent="0.3">
@@ -10604,7 +10576,7 @@
         <v>1015</v>
       </c>
       <c r="B1020" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1021" spans="1:2" x14ac:dyDescent="0.3">
@@ -10612,7 +10584,7 @@
         <v>1016</v>
       </c>
       <c r="B1021" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1022" spans="1:2" x14ac:dyDescent="0.3">
@@ -10620,7 +10592,7 @@
         <v>1017</v>
       </c>
       <c r="B1022" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1023" spans="1:2" x14ac:dyDescent="0.3">
@@ -10628,7 +10600,7 @@
         <v>1018</v>
       </c>
       <c r="B1023" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1024" spans="1:2" x14ac:dyDescent="0.3">
@@ -10636,7 +10608,7 @@
         <v>1019</v>
       </c>
       <c r="B1024" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.3">
@@ -10644,7 +10616,7 @@
         <v>1020</v>
       </c>
       <c r="B1025" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.3">
@@ -10652,7 +10624,7 @@
         <v>1021</v>
       </c>
       <c r="B1026" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.3">
@@ -10660,7 +10632,7 @@
         <v>1022</v>
       </c>
       <c r="B1027" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.3">
@@ -11055,47 +11027,47 @@
     </row>
     <row r="1106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1106" s="2" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1107" s="2" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1108" s="2" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1109" s="2" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1110" s="2" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1111" s="2" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1112" s="2" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="1113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1113" s="2" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1114" s="2" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>